<commit_message>
updated matches for district dc
</commit_message>
<xml_diff>
--- a/server/config/Matches.xlsx
+++ b/server/config/Matches.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rudic_000\workspace\FRC-Scouting\server\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rudic\frc\FRC-Scouting\server\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11660" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="matches" sheetId="1" r:id="rId1"/>
+    <sheet name="matches_champs" sheetId="1" r:id="rId1"/>
+    <sheet name="matches" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="209">
   <si>
     <t>Thu 8:30</t>
   </si>
@@ -412,12 +413,246 @@
   </si>
   <si>
     <t>BLUE</t>
+  </si>
+  <si>
+    <t>Sat 10:30 AM</t>
+  </si>
+  <si>
+    <t>Sat 10:38 AM</t>
+  </si>
+  <si>
+    <t>Sat 10:46 AM</t>
+  </si>
+  <si>
+    <t>Sat 10:57 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:05 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:13 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:21 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:29 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:37 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:48 AM</t>
+  </si>
+  <si>
+    <t>Sat 11:56 AM</t>
+  </si>
+  <si>
+    <t>Sat 12:04 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:12 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:20 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:28 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:39 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:47 PM</t>
+  </si>
+  <si>
+    <t>Sat 12:55 PM</t>
+  </si>
+  <si>
+    <t>Sat 1:03 PM</t>
+  </si>
+  <si>
+    <t>Sat 1:11 PM</t>
+  </si>
+  <si>
+    <t>Sat 1:49 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:00 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:08 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:16 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:24 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:32 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:40 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:51 PM</t>
+  </si>
+  <si>
+    <t>Sat 2:59 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:07 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:15 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:23 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:31 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:42 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:50 PM</t>
+  </si>
+  <si>
+    <t>Sat 3:58 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:06 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:14 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:22 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:33 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:41 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:49 PM</t>
+  </si>
+  <si>
+    <t>Sat 4:57 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:05 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:13 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:24 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:32 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:40 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:48 PM</t>
+  </si>
+  <si>
+    <t>Sat 5:56 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:04 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:15 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:23 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:31 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:39 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:47 PM</t>
+  </si>
+  <si>
+    <t>Sat 6:55 PM</t>
+  </si>
+  <si>
+    <t>Sat 7:06 PM</t>
+  </si>
+  <si>
+    <t>Sat 7:14 PM</t>
+  </si>
+  <si>
+    <t>Sat 7:22 PM</t>
+  </si>
+  <si>
+    <t>Sun 9:30 AM</t>
+  </si>
+  <si>
+    <t>Sun 9:38 AM</t>
+  </si>
+  <si>
+    <t>Sun 9:46 AM</t>
+  </si>
+  <si>
+    <t>Sun 9:57 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:05 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:13 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:21 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:29 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:37 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:48 AM</t>
+  </si>
+  <si>
+    <t>Sun 10:56 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:04 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:12 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:20 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:28 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:36 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:44 AM</t>
+  </si>
+  <si>
+    <t>Sun 11:52 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1034,6 +1269,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1069,6 +1321,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1223,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4547,6 +4816,2074 @@
       </c>
       <c r="H128">
         <v>4818</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4949</v>
+      </c>
+      <c r="D2">
+        <v>2963</v>
+      </c>
+      <c r="E2">
+        <v>3748</v>
+      </c>
+      <c r="F2">
+        <v>1885</v>
+      </c>
+      <c r="G2">
+        <v>3793</v>
+      </c>
+      <c r="H2">
+        <v>2186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3650</v>
+      </c>
+      <c r="D3">
+        <v>4242</v>
+      </c>
+      <c r="E3">
+        <v>5115</v>
+      </c>
+      <c r="F3">
+        <v>3283</v>
+      </c>
+      <c r="G3">
+        <v>2914</v>
+      </c>
+      <c r="H3">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4945</v>
+      </c>
+      <c r="D4">
+        <v>686</v>
+      </c>
+      <c r="E4">
+        <v>5569</v>
+      </c>
+      <c r="F4">
+        <v>4638</v>
+      </c>
+      <c r="G4">
+        <v>836</v>
+      </c>
+      <c r="H4">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2819</v>
+      </c>
+      <c r="D5">
+        <v>1418</v>
+      </c>
+      <c r="E5">
+        <v>1446</v>
+      </c>
+      <c r="F5">
+        <v>2849</v>
+      </c>
+      <c r="G5">
+        <v>4514</v>
+      </c>
+      <c r="H5">
+        <v>5979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2911</v>
+      </c>
+      <c r="D6">
+        <v>4464</v>
+      </c>
+      <c r="E6">
+        <v>5830</v>
+      </c>
+      <c r="F6">
+        <v>2964</v>
+      </c>
+      <c r="G6">
+        <v>4456</v>
+      </c>
+      <c r="H6">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2537</v>
+      </c>
+      <c r="D7">
+        <v>5587</v>
+      </c>
+      <c r="E7">
+        <v>1915</v>
+      </c>
+      <c r="F7">
+        <v>5549</v>
+      </c>
+      <c r="G7">
+        <v>2199</v>
+      </c>
+      <c r="H7">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>4821</v>
+      </c>
+      <c r="D8">
+        <v>5841</v>
+      </c>
+      <c r="E8">
+        <v>3748</v>
+      </c>
+      <c r="F8">
+        <v>2900</v>
+      </c>
+      <c r="G8">
+        <v>4242</v>
+      </c>
+      <c r="H8">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>3793</v>
+      </c>
+      <c r="D9">
+        <v>3283</v>
+      </c>
+      <c r="E9">
+        <v>2819</v>
+      </c>
+      <c r="F9">
+        <v>2911</v>
+      </c>
+      <c r="G9">
+        <v>2964</v>
+      </c>
+      <c r="H9">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>2912</v>
+      </c>
+      <c r="D10">
+        <v>686</v>
+      </c>
+      <c r="E10">
+        <v>1885</v>
+      </c>
+      <c r="F10">
+        <v>4099</v>
+      </c>
+      <c r="G10">
+        <v>1915</v>
+      </c>
+      <c r="H10">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5569</v>
+      </c>
+      <c r="D11">
+        <v>5587</v>
+      </c>
+      <c r="E11">
+        <v>2963</v>
+      </c>
+      <c r="F11">
+        <v>2914</v>
+      </c>
+      <c r="G11">
+        <v>5979</v>
+      </c>
+      <c r="H11">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>4945</v>
+      </c>
+      <c r="D12">
+        <v>2537</v>
+      </c>
+      <c r="E12">
+        <v>2186</v>
+      </c>
+      <c r="F12">
+        <v>4464</v>
+      </c>
+      <c r="G12">
+        <v>4821</v>
+      </c>
+      <c r="H12">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>449</v>
+      </c>
+      <c r="D13">
+        <v>4949</v>
+      </c>
+      <c r="E13">
+        <v>5115</v>
+      </c>
+      <c r="F13">
+        <v>2199</v>
+      </c>
+      <c r="G13">
+        <v>2849</v>
+      </c>
+      <c r="H13">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>3650</v>
+      </c>
+      <c r="D14">
+        <v>5830</v>
+      </c>
+      <c r="E14">
+        <v>836</v>
+      </c>
+      <c r="F14">
+        <v>4638</v>
+      </c>
+      <c r="G14">
+        <v>5549</v>
+      </c>
+      <c r="H14">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>5979</v>
+      </c>
+      <c r="D15">
+        <v>1915</v>
+      </c>
+      <c r="E15">
+        <v>2912</v>
+      </c>
+      <c r="F15">
+        <v>3283</v>
+      </c>
+      <c r="G15">
+        <v>4456</v>
+      </c>
+      <c r="H15">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>2819</v>
+      </c>
+      <c r="D16">
+        <v>2964</v>
+      </c>
+      <c r="E16">
+        <v>1885</v>
+      </c>
+      <c r="F16">
+        <v>4821</v>
+      </c>
+      <c r="G16">
+        <v>449</v>
+      </c>
+      <c r="H16">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>4638</v>
+      </c>
+      <c r="D17">
+        <v>2911</v>
+      </c>
+      <c r="E17">
+        <v>2537</v>
+      </c>
+      <c r="F17">
+        <v>5569</v>
+      </c>
+      <c r="G17">
+        <v>4514</v>
+      </c>
+      <c r="H17">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>4949</v>
+      </c>
+      <c r="D18">
+        <v>5549</v>
+      </c>
+      <c r="E18">
+        <v>5830</v>
+      </c>
+      <c r="F18">
+        <v>5115</v>
+      </c>
+      <c r="G18">
+        <v>1418</v>
+      </c>
+      <c r="H18">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>2186</v>
+      </c>
+      <c r="D19">
+        <v>2914</v>
+      </c>
+      <c r="E19">
+        <v>5587</v>
+      </c>
+      <c r="F19">
+        <v>2963</v>
+      </c>
+      <c r="G19">
+        <v>3793</v>
+      </c>
+      <c r="H19">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>4945</v>
+      </c>
+      <c r="D20">
+        <v>4242</v>
+      </c>
+      <c r="E20">
+        <v>4099</v>
+      </c>
+      <c r="F20">
+        <v>2849</v>
+      </c>
+      <c r="G20">
+        <v>686</v>
+      </c>
+      <c r="H20">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>3650</v>
+      </c>
+      <c r="D21">
+        <v>5841</v>
+      </c>
+      <c r="E21">
+        <v>4456</v>
+      </c>
+      <c r="F21">
+        <v>836</v>
+      </c>
+      <c r="G21">
+        <v>1418</v>
+      </c>
+      <c r="H21">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>2911</v>
+      </c>
+      <c r="D22">
+        <v>2819</v>
+      </c>
+      <c r="E22">
+        <v>5549</v>
+      </c>
+      <c r="F22">
+        <v>2186</v>
+      </c>
+      <c r="G22">
+        <v>5569</v>
+      </c>
+      <c r="H22">
+        <v>4638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>5979</v>
+      </c>
+      <c r="D23">
+        <v>4821</v>
+      </c>
+      <c r="E23">
+        <v>4242</v>
+      </c>
+      <c r="F23">
+        <v>3793</v>
+      </c>
+      <c r="G23">
+        <v>4514</v>
+      </c>
+      <c r="H23">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>1389</v>
+      </c>
+      <c r="D24">
+        <v>686</v>
+      </c>
+      <c r="E24">
+        <v>836</v>
+      </c>
+      <c r="F24">
+        <v>5587</v>
+      </c>
+      <c r="G24">
+        <v>4949</v>
+      </c>
+      <c r="H24">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>2849</v>
+      </c>
+      <c r="D25">
+        <v>2914</v>
+      </c>
+      <c r="E25">
+        <v>2912</v>
+      </c>
+      <c r="F25">
+        <v>2900</v>
+      </c>
+      <c r="G25">
+        <v>1885</v>
+      </c>
+      <c r="H25">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>449</v>
+      </c>
+      <c r="D26">
+        <v>2963</v>
+      </c>
+      <c r="E26">
+        <v>5830</v>
+      </c>
+      <c r="F26">
+        <v>3283</v>
+      </c>
+      <c r="G26">
+        <v>1446</v>
+      </c>
+      <c r="H26">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>4945</v>
+      </c>
+      <c r="D27">
+        <v>2199</v>
+      </c>
+      <c r="E27">
+        <v>3748</v>
+      </c>
+      <c r="F27">
+        <v>2964</v>
+      </c>
+      <c r="G27">
+        <v>3650</v>
+      </c>
+      <c r="H27">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>1418</v>
+      </c>
+      <c r="D28">
+        <v>2849</v>
+      </c>
+      <c r="E28">
+        <v>3793</v>
+      </c>
+      <c r="F28">
+        <v>4464</v>
+      </c>
+      <c r="G28">
+        <v>2900</v>
+      </c>
+      <c r="H28">
+        <v>2912</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>1885</v>
+      </c>
+      <c r="D29">
+        <v>1915</v>
+      </c>
+      <c r="E29">
+        <v>4638</v>
+      </c>
+      <c r="F29">
+        <v>4242</v>
+      </c>
+      <c r="G29">
+        <v>686</v>
+      </c>
+      <c r="H29">
+        <v>4949</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>2537</v>
+      </c>
+      <c r="D30">
+        <v>5569</v>
+      </c>
+      <c r="E30">
+        <v>5115</v>
+      </c>
+      <c r="F30">
+        <v>3748</v>
+      </c>
+      <c r="G30">
+        <v>5587</v>
+      </c>
+      <c r="H30">
+        <v>5830</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>5549</v>
+      </c>
+      <c r="D31">
+        <v>2963</v>
+      </c>
+      <c r="E31">
+        <v>4456</v>
+      </c>
+      <c r="F31">
+        <v>449</v>
+      </c>
+      <c r="G31">
+        <v>2819</v>
+      </c>
+      <c r="H31">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>3650</v>
+      </c>
+      <c r="D32">
+        <v>3283</v>
+      </c>
+      <c r="E32">
+        <v>4821</v>
+      </c>
+      <c r="F32">
+        <v>2199</v>
+      </c>
+      <c r="G32">
+        <v>5979</v>
+      </c>
+      <c r="H32">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>2964</v>
+      </c>
+      <c r="D33">
+        <v>5841</v>
+      </c>
+      <c r="E33">
+        <v>4514</v>
+      </c>
+      <c r="F33">
+        <v>1389</v>
+      </c>
+      <c r="G33">
+        <v>1446</v>
+      </c>
+      <c r="H33">
+        <v>4945</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>2914</v>
+      </c>
+      <c r="D34">
+        <v>449</v>
+      </c>
+      <c r="E34">
+        <v>4242</v>
+      </c>
+      <c r="F34">
+        <v>2911</v>
+      </c>
+      <c r="G34">
+        <v>2186</v>
+      </c>
+      <c r="H34">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>1418</v>
+      </c>
+      <c r="D35">
+        <v>4099</v>
+      </c>
+      <c r="E35">
+        <v>3748</v>
+      </c>
+      <c r="F35">
+        <v>3793</v>
+      </c>
+      <c r="G35">
+        <v>836</v>
+      </c>
+      <c r="H35">
+        <v>5587</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>1885</v>
+      </c>
+      <c r="D36">
+        <v>1446</v>
+      </c>
+      <c r="E36">
+        <v>5549</v>
+      </c>
+      <c r="F36">
+        <v>2819</v>
+      </c>
+      <c r="G36">
+        <v>2537</v>
+      </c>
+      <c r="H36">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>5115</v>
+      </c>
+      <c r="D37">
+        <v>2900</v>
+      </c>
+      <c r="E37">
+        <v>2199</v>
+      </c>
+      <c r="F37">
+        <v>4514</v>
+      </c>
+      <c r="G37">
+        <v>4638</v>
+      </c>
+      <c r="H37">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>2963</v>
+      </c>
+      <c r="D38">
+        <v>1389</v>
+      </c>
+      <c r="E38">
+        <v>5979</v>
+      </c>
+      <c r="F38">
+        <v>4945</v>
+      </c>
+      <c r="G38">
+        <v>2912</v>
+      </c>
+      <c r="H38">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>1915</v>
+      </c>
+      <c r="D39">
+        <v>2186</v>
+      </c>
+      <c r="E39">
+        <v>4464</v>
+      </c>
+      <c r="F39">
+        <v>2914</v>
+      </c>
+      <c r="G39">
+        <v>686</v>
+      </c>
+      <c r="H39">
+        <v>4821</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>5830</v>
+      </c>
+      <c r="D40">
+        <v>3283</v>
+      </c>
+      <c r="E40">
+        <v>2964</v>
+      </c>
+      <c r="F40">
+        <v>5841</v>
+      </c>
+      <c r="G40">
+        <v>4949</v>
+      </c>
+      <c r="H40">
+        <v>5569</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>4099</v>
+      </c>
+      <c r="D41">
+        <v>5115</v>
+      </c>
+      <c r="E41">
+        <v>2911</v>
+      </c>
+      <c r="F41">
+        <v>1418</v>
+      </c>
+      <c r="G41">
+        <v>2963</v>
+      </c>
+      <c r="H41">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>1389</v>
+      </c>
+      <c r="D42">
+        <v>4242</v>
+      </c>
+      <c r="E42">
+        <v>5549</v>
+      </c>
+      <c r="F42">
+        <v>1885</v>
+      </c>
+      <c r="G42">
+        <v>4456</v>
+      </c>
+      <c r="H42">
+        <v>4821</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>2914</v>
+      </c>
+      <c r="D43">
+        <v>4514</v>
+      </c>
+      <c r="E43">
+        <v>2900</v>
+      </c>
+      <c r="F43">
+        <v>2964</v>
+      </c>
+      <c r="G43">
+        <v>1915</v>
+      </c>
+      <c r="H43">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>3793</v>
+      </c>
+      <c r="D44">
+        <v>3748</v>
+      </c>
+      <c r="E44">
+        <v>2912</v>
+      </c>
+      <c r="F44">
+        <v>2849</v>
+      </c>
+      <c r="G44">
+        <v>5569</v>
+      </c>
+      <c r="H44">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>174</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>2186</v>
+      </c>
+      <c r="D45">
+        <v>5979</v>
+      </c>
+      <c r="E45">
+        <v>5841</v>
+      </c>
+      <c r="F45">
+        <v>5830</v>
+      </c>
+      <c r="G45">
+        <v>2819</v>
+      </c>
+      <c r="H45">
+        <v>2199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>4638</v>
+      </c>
+      <c r="D46">
+        <v>1446</v>
+      </c>
+      <c r="E46">
+        <v>4464</v>
+      </c>
+      <c r="F46">
+        <v>2537</v>
+      </c>
+      <c r="G46">
+        <v>3283</v>
+      </c>
+      <c r="H46">
+        <v>4949</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>686</v>
+      </c>
+      <c r="D47">
+        <v>5587</v>
+      </c>
+      <c r="E47">
+        <v>449</v>
+      </c>
+      <c r="F47">
+        <v>4945</v>
+      </c>
+      <c r="G47">
+        <v>2914</v>
+      </c>
+      <c r="H47">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>177</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>836</v>
+      </c>
+      <c r="D48">
+        <v>2912</v>
+      </c>
+      <c r="E48">
+        <v>4821</v>
+      </c>
+      <c r="F48">
+        <v>1389</v>
+      </c>
+      <c r="G48">
+        <v>3748</v>
+      </c>
+      <c r="H48">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>1446</v>
+      </c>
+      <c r="D49">
+        <v>2849</v>
+      </c>
+      <c r="E49">
+        <v>4949</v>
+      </c>
+      <c r="F49">
+        <v>5830</v>
+      </c>
+      <c r="G49">
+        <v>2537</v>
+      </c>
+      <c r="H49">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>2900</v>
+      </c>
+      <c r="D50">
+        <v>2964</v>
+      </c>
+      <c r="E50">
+        <v>5569</v>
+      </c>
+      <c r="F50">
+        <v>5587</v>
+      </c>
+      <c r="G50">
+        <v>1885</v>
+      </c>
+      <c r="H50">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>686</v>
+      </c>
+      <c r="D51">
+        <v>5979</v>
+      </c>
+      <c r="E51">
+        <v>4638</v>
+      </c>
+      <c r="F51">
+        <v>2186</v>
+      </c>
+      <c r="G51">
+        <v>3283</v>
+      </c>
+      <c r="H51">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>4456</v>
+      </c>
+      <c r="D52">
+        <v>3793</v>
+      </c>
+      <c r="E52">
+        <v>2911</v>
+      </c>
+      <c r="F52">
+        <v>1915</v>
+      </c>
+      <c r="G52">
+        <v>4945</v>
+      </c>
+      <c r="H52">
+        <v>5549</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>4514</v>
+      </c>
+      <c r="D53">
+        <v>2199</v>
+      </c>
+      <c r="E53">
+        <v>4242</v>
+      </c>
+      <c r="F53">
+        <v>5841</v>
+      </c>
+      <c r="G53">
+        <v>2963</v>
+      </c>
+      <c r="H53">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>2912</v>
+      </c>
+      <c r="D54">
+        <v>5587</v>
+      </c>
+      <c r="E54">
+        <v>1389</v>
+      </c>
+      <c r="F54">
+        <v>4949</v>
+      </c>
+      <c r="G54">
+        <v>2819</v>
+      </c>
+      <c r="H54">
+        <v>4638</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>2186</v>
+      </c>
+      <c r="D55">
+        <v>1446</v>
+      </c>
+      <c r="E55">
+        <v>5115</v>
+      </c>
+      <c r="F55">
+        <v>2900</v>
+      </c>
+      <c r="G55">
+        <v>1915</v>
+      </c>
+      <c r="H55">
+        <v>2911</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>5979</v>
+      </c>
+      <c r="D56">
+        <v>4464</v>
+      </c>
+      <c r="E56">
+        <v>1885</v>
+      </c>
+      <c r="F56">
+        <v>3793</v>
+      </c>
+      <c r="G56">
+        <v>4099</v>
+      </c>
+      <c r="H56">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>5830</v>
+      </c>
+      <c r="D57">
+        <v>1418</v>
+      </c>
+      <c r="E57">
+        <v>5569</v>
+      </c>
+      <c r="F57">
+        <v>4945</v>
+      </c>
+      <c r="G57">
+        <v>4821</v>
+      </c>
+      <c r="H57">
+        <v>2963</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>4242</v>
+      </c>
+      <c r="D58">
+        <v>836</v>
+      </c>
+      <c r="E58">
+        <v>4456</v>
+      </c>
+      <c r="F58">
+        <v>2964</v>
+      </c>
+      <c r="G58">
+        <v>2537</v>
+      </c>
+      <c r="H58">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>4514</v>
+      </c>
+      <c r="D59">
+        <v>3283</v>
+      </c>
+      <c r="E59">
+        <v>686</v>
+      </c>
+      <c r="F59">
+        <v>5549</v>
+      </c>
+      <c r="G59">
+        <v>3748</v>
+      </c>
+      <c r="H59">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>3650</v>
+      </c>
+      <c r="D60">
+        <v>2199</v>
+      </c>
+      <c r="E60">
+        <v>4638</v>
+      </c>
+      <c r="F60">
+        <v>2914</v>
+      </c>
+      <c r="G60">
+        <v>5830</v>
+      </c>
+      <c r="H60">
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>2900</v>
+      </c>
+      <c r="D61">
+        <v>836</v>
+      </c>
+      <c r="E61">
+        <v>4949</v>
+      </c>
+      <c r="F61">
+        <v>4242</v>
+      </c>
+      <c r="G61">
+        <v>2963</v>
+      </c>
+      <c r="H61">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>4099</v>
+      </c>
+      <c r="D62">
+        <v>2912</v>
+      </c>
+      <c r="E62">
+        <v>3283</v>
+      </c>
+      <c r="F62">
+        <v>2186</v>
+      </c>
+      <c r="G62">
+        <v>4514</v>
+      </c>
+      <c r="H62">
+        <v>4821</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <v>1915</v>
+      </c>
+      <c r="D63">
+        <v>4456</v>
+      </c>
+      <c r="E63">
+        <v>2849</v>
+      </c>
+      <c r="F63">
+        <v>5569</v>
+      </c>
+      <c r="G63">
+        <v>1389</v>
+      </c>
+      <c r="H63">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>193</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <v>3748</v>
+      </c>
+      <c r="D64">
+        <v>449</v>
+      </c>
+      <c r="E64">
+        <v>2911</v>
+      </c>
+      <c r="F64">
+        <v>1418</v>
+      </c>
+      <c r="G64">
+        <v>5587</v>
+      </c>
+      <c r="H64">
+        <v>5841</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <v>2537</v>
+      </c>
+      <c r="D65">
+        <v>2199</v>
+      </c>
+      <c r="E65">
+        <v>2914</v>
+      </c>
+      <c r="F65">
+        <v>5115</v>
+      </c>
+      <c r="G65">
+        <v>2819</v>
+      </c>
+      <c r="H65">
+        <v>4945</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <v>1446</v>
+      </c>
+      <c r="D66">
+        <v>2964</v>
+      </c>
+      <c r="E66">
+        <v>5979</v>
+      </c>
+      <c r="F66">
+        <v>686</v>
+      </c>
+      <c r="G66">
+        <v>5549</v>
+      </c>
+      <c r="H66">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <v>2900</v>
+      </c>
+      <c r="D67">
+        <v>4821</v>
+      </c>
+      <c r="E67">
+        <v>4099</v>
+      </c>
+      <c r="F67">
+        <v>2911</v>
+      </c>
+      <c r="G67">
+        <v>3283</v>
+      </c>
+      <c r="H67">
+        <v>5587</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <v>449</v>
+      </c>
+      <c r="D68">
+        <v>1885</v>
+      </c>
+      <c r="E68">
+        <v>4514</v>
+      </c>
+      <c r="F68">
+        <v>4456</v>
+      </c>
+      <c r="G68">
+        <v>2186</v>
+      </c>
+      <c r="H68">
+        <v>5830</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>198</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <v>2914</v>
+      </c>
+      <c r="D69">
+        <v>1915</v>
+      </c>
+      <c r="E69">
+        <v>4949</v>
+      </c>
+      <c r="F69">
+        <v>1418</v>
+      </c>
+      <c r="G69">
+        <v>5979</v>
+      </c>
+      <c r="H69">
+        <v>5549</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>199</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <v>3650</v>
+      </c>
+      <c r="D70">
+        <v>4464</v>
+      </c>
+      <c r="E70">
+        <v>3793</v>
+      </c>
+      <c r="F70">
+        <v>2819</v>
+      </c>
+      <c r="G70">
+        <v>5569</v>
+      </c>
+      <c r="H70">
+        <v>4242</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <v>686</v>
+      </c>
+      <c r="D71">
+        <v>2537</v>
+      </c>
+      <c r="E71">
+        <v>5841</v>
+      </c>
+      <c r="F71">
+        <v>2912</v>
+      </c>
+      <c r="G71">
+        <v>5115</v>
+      </c>
+      <c r="H71">
+        <v>2963</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>201</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <v>2849</v>
+      </c>
+      <c r="D72">
+        <v>1389</v>
+      </c>
+      <c r="E72">
+        <v>4638</v>
+      </c>
+      <c r="F72">
+        <v>836</v>
+      </c>
+      <c r="G72">
+        <v>3748</v>
+      </c>
+      <c r="H72">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>202</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <v>4945</v>
+      </c>
+      <c r="D73">
+        <v>4514</v>
+      </c>
+      <c r="E73">
+        <v>1418</v>
+      </c>
+      <c r="F73">
+        <v>2199</v>
+      </c>
+      <c r="G73">
+        <v>2964</v>
+      </c>
+      <c r="H73">
+        <v>4949</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <v>3650</v>
+      </c>
+      <c r="D74">
+        <v>5549</v>
+      </c>
+      <c r="E74">
+        <v>5587</v>
+      </c>
+      <c r="F74">
+        <v>5841</v>
+      </c>
+      <c r="G74">
+        <v>2912</v>
+      </c>
+      <c r="H74">
+        <v>4242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>204</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <v>2186</v>
+      </c>
+      <c r="D75">
+        <v>836</v>
+      </c>
+      <c r="E75">
+        <v>2819</v>
+      </c>
+      <c r="F75">
+        <v>5830</v>
+      </c>
+      <c r="G75">
+        <v>1915</v>
+      </c>
+      <c r="H75">
+        <v>5115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>205</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <v>3283</v>
+      </c>
+      <c r="D76">
+        <v>4945</v>
+      </c>
+      <c r="E76">
+        <v>4464</v>
+      </c>
+      <c r="F76">
+        <v>2914</v>
+      </c>
+      <c r="G76">
+        <v>3748</v>
+      </c>
+      <c r="H76">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <v>2537</v>
+      </c>
+      <c r="D77">
+        <v>1389</v>
+      </c>
+      <c r="E77">
+        <v>2900</v>
+      </c>
+      <c r="F77">
+        <v>3793</v>
+      </c>
+      <c r="G77">
+        <v>449</v>
+      </c>
+      <c r="H77">
+        <v>5979</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <v>2849</v>
+      </c>
+      <c r="D78">
+        <v>2963</v>
+      </c>
+      <c r="E78">
+        <v>4099</v>
+      </c>
+      <c r="F78">
+        <v>4821</v>
+      </c>
+      <c r="G78">
+        <v>4638</v>
+      </c>
+      <c r="H78">
+        <v>2964</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>208</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <v>4456</v>
+      </c>
+      <c r="D79">
+        <v>2199</v>
+      </c>
+      <c r="E79">
+        <v>5569</v>
+      </c>
+      <c r="F79">
+        <v>1446</v>
+      </c>
+      <c r="G79">
+        <v>686</v>
+      </c>
+      <c r="H79">
+        <v>2911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>